<commit_message>
added modified problem3 results to the spreadsheet showing heuristic superiority
</commit_message>
<xml_diff>
--- a/aind_planning_analysis.xlsx
+++ b/aind_planning_analysis.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deran/PycharmProjects/AIND-Planning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donay\PycharmProjects\AIND-Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="980" yWindow="460" windowWidth="29020" windowHeight="20540" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="1905" yWindow="465" windowWidth="29025" windowHeight="20535" tabRatio="841" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="stats" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,9 @@
     <sheet name="domain independent heuristics" sheetId="4" r:id="rId4"/>
     <sheet name="heuristic comparison" sheetId="5" r:id="rId5"/>
     <sheet name="heuristics_vs_uninformed" sheetId="6" r:id="rId6"/>
+    <sheet name="problem3_modified" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="65">
   <si>
     <t>breadth_first_search</t>
   </si>
@@ -225,18 +226,27 @@
   <si>
     <t>Problem-3</t>
   </si>
+  <si>
+    <t>Problem-4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -290,28 +300,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="10">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -321,6 +335,7 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="9"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -328,12 +343,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -407,23 +425,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>56.0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>180.0</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0234</c:v>
+                  <c:v>2.3400000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B9D5-461C-9974-DF64A83158C8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -479,23 +502,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>21.0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>84.0</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0098</c:v>
+                  <c:v>9.7999999999999997E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B9D5-461C-9974-DF64A83158C8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -551,23 +579,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>55.0</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>57.0</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>224.0</c:v>
+                  <c:v>224</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0339</c:v>
+                  <c:v>3.39E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B9D5-461C-9974-DF64A83158C8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -774,7 +807,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -848,23 +881,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3343.0</c:v>
+                  <c:v>3343</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4609.0</c:v>
+                  <c:v>4609</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30509.0</c:v>
+                  <c:v>30509</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.7725</c:v>
+                  <c:v>10.772500000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9973-409E-88AE-DCCCC3D76B10}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -920,16 +958,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>624.0</c:v>
+                  <c:v>624</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>625.0</c:v>
+                  <c:v>625</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5602.0</c:v>
+                  <c:v>5602</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>619.0</c:v>
+                  <c:v>619</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>3.1698</c:v>
@@ -937,6 +975,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9973-409E-88AE-DCCCC3D76B10}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -992,23 +1035,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>4853.0</c:v>
+                  <c:v>4853</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4855.0</c:v>
+                  <c:v>4855</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44041.0</c:v>
+                  <c:v>44041</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.0829</c:v>
+                  <c:v>8.0829000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9973-409E-88AE-DCCCC3D76B10}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1215,7 +1263,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1289,23 +1337,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>14663.0</c:v>
+                  <c:v>14663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18098.0</c:v>
+                  <c:v>18098</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>129631.0</c:v>
+                  <c:v>129631</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>90.786</c:v>
+                  <c:v>90.786000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-93BE-405D-872F-E470F2B53AB4}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1361,23 +1414,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>408.0</c:v>
+                  <c:v>408</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>409.0</c:v>
+                  <c:v>409</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3364.0</c:v>
+                  <c:v>3364</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>392.0</c:v>
+                  <c:v>392</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3755</c:v>
+                  <c:v>1.3754999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-93BE-405D-872F-E470F2B53AB4}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1433,23 +1491,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>18151.0</c:v>
+                  <c:v>18151</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18153.0</c:v>
+                  <c:v>18153</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>159038.0</c:v>
+                  <c:v>159038</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>33.8472</c:v>
+                  <c:v>33.847200000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-93BE-405D-872F-E470F2B53AB4}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1656,7 +1719,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1730,23 +1793,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>41.0</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43.0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>170.0</c:v>
+                  <c:v>170</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0915</c:v>
+                  <c:v>9.1499999999999998E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8952-40A1-A24C-CDA39A38DB59}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1802,23 +1870,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.7812</c:v>
+                  <c:v>0.78120000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8952-40A1-A24C-CDA39A38DB59}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2025,7 +2098,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2099,23 +2172,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1450.0</c:v>
+                  <c:v>1450</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1452.0</c:v>
+                  <c:v>1452</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13303.0</c:v>
+                  <c:v>13303</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>33.101</c:v>
+                  <c:v>33.100999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C1A5-4877-8C89-B267C69C1DE1}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2171,23 +2249,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>86.0</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>88.0</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>841.0</c:v>
+                  <c:v>841</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>66.9705</c:v>
+                  <c:v>66.970500000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C1A5-4877-8C89-B267C69C1DE1}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2394,7 +2477,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2468,23 +2551,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5038.0</c:v>
+                  <c:v>5038</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5040.0</c:v>
+                  <c:v>5040</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44926.0</c:v>
+                  <c:v>44926</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>181.2812</c:v>
+                  <c:v>181.28120000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DB31-4DE3-A19B-F557A1F6BAE7}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2540,23 +2628,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>293.0</c:v>
+                  <c:v>293</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>295.0</c:v>
+                  <c:v>295</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2694.0</c:v>
+                  <c:v>2694</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>298.951</c:v>
+                  <c:v>298.95100000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DB31-4DE3-A19B-F557A1F6BAE7}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2763,7 +2856,7 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2832,18 +2925,23 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-49DC-488B-94DD-C3F7B000309E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2895,18 +2993,23 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>8.537704918032787</c:v>
+                  <c:v>8.5377049180327873</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.023216821244071</c:v>
+                  <c:v>2.0232168212440711</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.649100954759787</c:v>
+                  <c:v>1.6491009547597875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-49DC-488B-94DD-C3F7B000309E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3037,7 +3140,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3105,7 +3207,7 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3119,7 +3221,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3205,18 +3306,23 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-13BA-4064-8528-AB79025A77D7}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3268,18 +3374,23 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>33.38461538461539</c:v>
+                  <c:v>33.384615384615387</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.216802042237177</c:v>
+                  <c:v>6.2168020422371777</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.292919613156214</c:v>
+                  <c:v>3.2929196131562137</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-13BA-4064-8528-AB79025A77D7}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3410,7 +3521,443 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
       <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>problem3_modified!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>breadth_first_search</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>problem3_modified!$B$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Problem-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Problem-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Problem-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Problem-4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>problem3_modified!$B$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.3400000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.772500000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90.786000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3668</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7B09-4C3D-8F91-FB77DB7C55D4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>problem3_modified!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>depth_first_graph_search</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>problem3_modified!$B$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Problem-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Problem-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Problem-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Problem-4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>problem3_modified!$B$3:$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>9.7999999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.1698</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3754999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1565</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7B09-4C3D-8F91-FB77DB7C55D4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>problem3_modified!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>h_pg_levelsum</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>problem3_modified!$B$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Problem-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Problem-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Problem-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Problem-4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>problem3_modified!$B$4:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.78120000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>66.970500000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>298.95100000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>780</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7B09-4C3D-8F91-FB77DB7C55D4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="333891992"/>
+        <c:axId val="333898880"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="333891992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="333898880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="333898880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="333891992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3797,6 +4344,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
@@ -7333,6 +7920,511 @@
 </file>
 
 <file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7854,7 +8946,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7884,7 +8982,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -7916,7 +9020,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -7953,7 +9063,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -7985,7 +9101,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -8017,7 +9139,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -8054,7 +9182,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8089,7 +9223,54 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60C8F18B-90CE-49D2-9851-95ADDAA3061E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8376,47 +9557,47 @@
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="G1" s="3" t="s">
+    <row r="1" spans="1:9">
+      <c r="G1" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>14</v>
       </c>
       <c r="I2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:9">
+      <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B3">
@@ -8425,304 +9606,304 @@
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>40</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>56</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>180</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>6</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <v>2.3400000000000001E-2</v>
       </c>
       <c r="I3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
+    <row r="4" spans="1:9">
+      <c r="A4" s="5"/>
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>1458</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>1459</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>5960</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>6</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <v>0.63119999999999998</v>
       </c>
       <c r="I4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
+    <row r="5" spans="1:9">
+      <c r="A5" s="5"/>
       <c r="B5">
         <v>3</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>21</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>22</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>84</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>20</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <v>9.7999999999999997E-3</v>
       </c>
       <c r="I5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
+    <row r="6" spans="1:9">
+      <c r="A6" s="5"/>
       <c r="B6">
         <v>4</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>101</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>271</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>414</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>50</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <v>6.9099999999999995E-2</v>
       </c>
       <c r="I6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
+    <row r="7" spans="1:9">
+      <c r="A7" s="5"/>
       <c r="B7">
         <v>5</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>55</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>57</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>224</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>6</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <v>3.39E-2</v>
       </c>
       <c r="I7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
+    <row r="8" spans="1:9">
+      <c r="A8" s="5"/>
       <c r="B8">
         <v>6</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>4229</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>4230</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>17023</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>6</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <v>1.8794</v>
       </c>
       <c r="I8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
+    <row r="9" spans="1:9">
+      <c r="A9" s="5"/>
       <c r="B9">
         <v>7</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>7</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>9</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>28</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>6</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
         <v>3.5000000000000001E-3</v>
       </c>
       <c r="I9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
+    <row r="10" spans="1:9">
+      <c r="A10" s="5"/>
       <c r="B10">
         <v>8</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>55</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>57</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>224</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>6</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="3">
         <v>3.3099999999999997E-2</v>
       </c>
       <c r="I10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
+    <row r="11" spans="1:9">
+      <c r="A11" s="5"/>
       <c r="B11">
         <v>9</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>41</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>43</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>170</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <v>6</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="3">
         <v>9.1499999999999998E-2</v>
       </c>
       <c r="I11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
+    <row r="12" spans="1:9">
+      <c r="A12" s="5"/>
       <c r="B12">
         <v>10</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>10</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>12</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <v>48</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <v>6</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="3">
         <v>0.78120000000000001</v>
       </c>
       <c r="I12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+    <row r="13" spans="1:9">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="B14" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="3" t="s">
         <v>14</v>
       </c>
       <c r="I14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:9">
+      <c r="A15" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B15">
@@ -8731,271 +9912,271 @@
       <c r="C15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <v>3343</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>4609</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="3">
         <v>30509</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <v>9</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="3">
         <v>10.772500000000001</v>
       </c>
       <c r="I15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
+    <row r="16" spans="1:9">
+      <c r="A16" s="5"/>
       <c r="B16">
         <v>2</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4">
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3">
         <v>600</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
+    <row r="17" spans="1:9">
+      <c r="A17" s="5"/>
       <c r="B17">
         <v>3</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <v>624</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>625</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <v>5602</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <v>619</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="3">
         <v>3.1698</v>
       </c>
       <c r="I17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
+    <row r="18" spans="1:9">
+      <c r="A18" s="5"/>
       <c r="B18">
         <v>4</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4">
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3">
         <v>600</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
+    <row r="19" spans="1:9">
+      <c r="A19" s="5"/>
       <c r="B19">
         <v>5</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="3">
         <v>4853</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="3">
         <v>4855</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="3">
         <v>44041</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="3">
         <v>9</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H19" s="3">
         <v>8.0829000000000004</v>
       </c>
       <c r="I19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
+    <row r="20" spans="1:9">
+      <c r="A20" s="5"/>
       <c r="B20">
         <v>6</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4">
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3">
         <v>600</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
+    <row r="21" spans="1:9">
+      <c r="A21" s="5"/>
       <c r="B21">
         <v>7</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="3">
         <v>998</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="3">
         <v>1000</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="3">
         <v>8982</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="3">
         <v>17</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21" s="3">
         <v>1.4893000000000001</v>
       </c>
       <c r="I21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
+    <row r="22" spans="1:9">
+      <c r="A22" s="5"/>
       <c r="B22">
         <v>8</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="3">
         <v>4853</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="3">
         <v>4855</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="3">
         <v>44041</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="3">
         <v>9</v>
       </c>
-      <c r="H22" s="4">
+      <c r="H22" s="3">
         <v>7.9112</v>
       </c>
       <c r="I22" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
+    <row r="23" spans="1:9">
+      <c r="A23" s="5"/>
       <c r="B23">
         <v>9</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="3">
         <v>1450</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="3">
         <v>1452</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="3">
         <v>13303</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="3">
         <v>9</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H23" s="3">
         <v>33.100999999999999</v>
       </c>
       <c r="I23" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
+    <row r="24" spans="1:9">
+      <c r="A24" s="5"/>
       <c r="B24">
         <v>10</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="3">
         <v>86</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="3">
         <v>88</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F24" s="3">
         <v>841</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="3">
         <v>9</v>
       </c>
-      <c r="H24" s="4">
+      <c r="H24" s="3">
         <v>66.970500000000001</v>
       </c>
       <c r="I24" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
+    <row r="25" spans="1:9">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="B26" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="G26" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="H26" s="3" t="s">
         <v>14</v>
       </c>
       <c r="I26" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:9">
+      <c r="A27" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B27">
@@ -9004,229 +10185,229 @@
       <c r="C27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D27" s="3">
         <v>14663</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="3">
         <v>18098</v>
       </c>
-      <c r="F27" s="4">
+      <c r="F27" s="3">
         <v>129631</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27" s="3">
         <v>12</v>
       </c>
-      <c r="H27" s="4">
+      <c r="H27" s="3">
         <v>90.786000000000001</v>
       </c>
       <c r="I27" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
+    <row r="28" spans="1:9">
+      <c r="A28" s="5"/>
       <c r="B28">
         <v>2</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4">
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3">
         <v>600</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
+    <row r="29" spans="1:9">
+      <c r="A29" s="5"/>
       <c r="B29">
         <v>3</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="3">
         <v>408</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="3">
         <v>409</v>
       </c>
-      <c r="F29" s="4">
+      <c r="F29" s="3">
         <v>3364</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="3">
         <v>392</v>
       </c>
-      <c r="H29" s="4">
+      <c r="H29" s="3">
         <v>1.3754999999999999</v>
       </c>
       <c r="I29" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
+    <row r="30" spans="1:9">
+      <c r="A30" s="5"/>
       <c r="B30">
         <v>4</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4">
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3">
         <v>600</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
+    <row r="31" spans="1:9">
+      <c r="A31" s="5"/>
       <c r="B31">
         <v>5</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="3">
         <v>18151</v>
       </c>
-      <c r="E31" s="4">
+      <c r="E31" s="3">
         <v>18153</v>
       </c>
-      <c r="F31" s="4">
+      <c r="F31" s="3">
         <v>159038</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G31" s="3">
         <v>12</v>
       </c>
-      <c r="H31" s="4">
+      <c r="H31" s="3">
         <v>33.847200000000001</v>
       </c>
       <c r="I31" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
+    <row r="32" spans="1:9">
+      <c r="A32" s="5"/>
       <c r="B32">
         <v>6</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4">
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3">
         <v>600</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
+    <row r="33" spans="1:9">
+      <c r="A33" s="5"/>
       <c r="B33">
         <v>7</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D33" s="3">
         <v>5398</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E33" s="3">
         <v>5400</v>
       </c>
-      <c r="F33" s="4">
+      <c r="F33" s="3">
         <v>47665</v>
       </c>
-      <c r="G33" s="4">
+      <c r="G33" s="3">
         <v>26</v>
       </c>
-      <c r="H33" s="4">
+      <c r="H33" s="3">
         <v>10.021000000000001</v>
       </c>
       <c r="I33" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
+    <row r="34" spans="1:9">
+      <c r="A34" s="5"/>
       <c r="B34">
         <v>8</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D34" s="3">
         <v>18151</v>
       </c>
-      <c r="E34" s="4">
+      <c r="E34" s="3">
         <v>18153</v>
       </c>
-      <c r="F34" s="4">
+      <c r="F34" s="3">
         <v>159038</v>
       </c>
-      <c r="G34" s="4">
+      <c r="G34" s="3">
         <v>12</v>
       </c>
-      <c r="H34" s="4">
+      <c r="H34" s="3">
         <v>33.648099999999999</v>
       </c>
       <c r="I34" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
+    <row r="35" spans="1:9">
+      <c r="A35" s="5"/>
       <c r="B35">
         <v>9</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D35" s="3">
         <v>5038</v>
       </c>
-      <c r="E35" s="4">
+      <c r="E35" s="3">
         <v>5040</v>
       </c>
-      <c r="F35" s="4">
+      <c r="F35" s="3">
         <v>44926</v>
       </c>
-      <c r="G35" s="4">
+      <c r="G35" s="3">
         <v>12</v>
       </c>
-      <c r="H35" s="4">
+      <c r="H35" s="3">
         <v>181.28120000000001</v>
       </c>
       <c r="I35" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
+    <row r="36" spans="1:9">
+      <c r="A36" s="5"/>
       <c r="B36">
         <v>10</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D36" s="3">
         <v>293</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E36" s="3">
         <v>295</v>
       </c>
-      <c r="F36" s="4">
+      <c r="F36" s="3">
         <v>2694</v>
       </c>
-      <c r="G36" s="4">
+      <c r="G36" s="3">
         <v>12</v>
       </c>
-      <c r="H36" s="4">
+      <c r="H36" s="3">
         <v>298.95100000000002</v>
       </c>
       <c r="I36" t="s">
@@ -9252,14 +10433,14 @@
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -9285,7 +10466,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -9311,7 +10492,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -9337,7 +10518,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -9363,7 +10544,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -9371,7 +10552,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -9379,7 +10560,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -9387,7 +10568,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -9405,304 +10586,304 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F1" sqref="A1:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>40</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>56</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>180</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>6</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>2.3400000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:6">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>21</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>22</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>84</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>20</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>9.7999999999999997E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:6">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>55</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>57</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>224</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>6</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>3.39E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+    <row r="5" spans="1:6">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+    <row r="7" spans="1:6">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:6">
+      <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:6">
+      <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>3343</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>4609</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>30509</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>9</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>10.772500000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:6">
+      <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>624</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>625</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>5602</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>619</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>3.1698</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:6">
+      <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>4853</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>4855</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>44041</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>9</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>8.0829000000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
+    <row r="12" spans="1:6">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+    <row r="13" spans="1:6">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
+    <row r="14" spans="1:6">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:6">
+      <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+    <row r="16" spans="1:6">
+      <c r="A16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>14663</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <v>18098</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <v>129631</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <v>12</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="3">
         <v>90.786000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:6">
+      <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <v>408</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>409</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <v>3364</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>392</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <v>1.3754999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:6">
+      <c r="A18" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <v>18151</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <v>18153</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="3">
         <v>159038</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="3">
         <v>12</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="3">
         <v>33.847200000000001</v>
       </c>
     </row>
@@ -9720,265 +10901,265 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>41</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>43</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>170</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>6</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>9.1499999999999998E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:6">
+      <c r="A3" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>10</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>12</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>48</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>6</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>0.78120000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+    <row r="4" spans="1:6">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+    <row r="5" spans="1:6">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+    <row r="7" spans="1:6">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+    <row r="8" spans="1:6">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:6">
+      <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:6">
+      <c r="A10" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>1450</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>1452</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>13303</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>9</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>33.100999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:6">
+      <c r="A11" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>86</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>88</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>841</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>9</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>66.970500000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
+    <row r="12" spans="1:6">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+    <row r="13" spans="1:6">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
+    <row r="14" spans="1:6">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+    <row r="15" spans="1:6">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:6">
+      <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:6">
+      <c r="A17" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <v>5038</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>5040</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <v>44926</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>12</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <v>181.28120000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:6">
+      <c r="A18" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <v>293</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <v>295</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="3">
         <v>2694</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="3">
         <v>12</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="3">
         <v>298.95100000000002</v>
       </c>
     </row>
@@ -9993,16 +11174,16 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="B3:D3"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="B1" t="s">
         <v>61</v>
       </c>
@@ -10022,21 +11203,21 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:9">
+      <c r="A2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>9.1499999999999998E-2</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>33.100999999999999</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>181.28120000000001</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
         <v>59</v>
       </c>
       <c r="G2">
@@ -10052,21 +11233,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:9">
+      <c r="A3" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>0.78120000000000001</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>66.970500000000001</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>298.95100000000002</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4" t="s">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
         <v>60</v>
       </c>
       <c r="G3">
@@ -10092,17 +11273,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="B2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="B1" t="s">
         <v>61</v>
       </c>
@@ -10122,46 +11303,46 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:9">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>2.3400000000000001E-2</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>10.772500000000001</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>90.786000000000001</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>1</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <v>1</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:9">
+      <c r="A3" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>0.78120000000000001</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>66.970500000000001</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>298.95100000000002</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>60</v>
       </c>
       <c r="G3">
@@ -10181,4 +11362,397 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="19.25" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8">
+        <v>2.3400000000000001E-2</v>
+      </c>
+      <c r="C2" s="8">
+        <v>10.772500000000001</v>
+      </c>
+      <c r="D2" s="8">
+        <v>90.786000000000001</v>
+      </c>
+      <c r="E2" s="7">
+        <v>3668</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="8">
+        <v>1</v>
+      </c>
+      <c r="I2" s="8">
+        <v>1</v>
+      </c>
+      <c r="J2" s="8">
+        <v>1</v>
+      </c>
+      <c r="K2" s="7">
+        <v>1</v>
+      </c>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8">
+        <v>9.7999999999999997E-3</v>
+      </c>
+      <c r="C3" s="8">
+        <v>3.1698</v>
+      </c>
+      <c r="D3" s="8">
+        <v>1.3754999999999999</v>
+      </c>
+      <c r="E3" s="7">
+        <v>1565</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="8">
+        <f>B3/B2</f>
+        <v>0.41880341880341876</v>
+      </c>
+      <c r="I3" s="8">
+        <f t="shared" ref="I3:K3" si="0">C3/C2</f>
+        <v>0.29424924576467854</v>
+      </c>
+      <c r="J3" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5151014473597249E-2</v>
+      </c>
+      <c r="K3" s="8">
+        <f t="shared" si="0"/>
+        <v>0.42666303162486369</v>
+      </c>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="8">
+        <v>0.78120000000000001</v>
+      </c>
+      <c r="C4" s="8">
+        <v>66.970500000000001</v>
+      </c>
+      <c r="D4" s="8">
+        <v>298.95100000000002</v>
+      </c>
+      <c r="E4" s="7">
+        <v>780</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="8">
+        <f>B4/B2</f>
+        <v>33.384615384615387</v>
+      </c>
+      <c r="I4" s="8">
+        <f t="shared" ref="I4:K4" si="1">C4/C2</f>
+        <v>6.2168020422371777</v>
+      </c>
+      <c r="J4" s="8">
+        <f t="shared" si="1"/>
+        <v>3.2929196131562137</v>
+      </c>
+      <c r="K4" s="8">
+        <f t="shared" si="1"/>
+        <v>0.21264994547437296</v>
+      </c>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="8">
+        <v>112090</v>
+      </c>
+      <c r="C12" s="8">
+        <v>121416</v>
+      </c>
+      <c r="D12" s="8">
+        <v>1055564</v>
+      </c>
+      <c r="E12" s="8">
+        <v>15</v>
+      </c>
+      <c r="F12" s="7">
+        <v>3668</v>
+      </c>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="8">
+        <v>15450</v>
+      </c>
+      <c r="C13" s="8">
+        <v>15451</v>
+      </c>
+      <c r="D13" s="8">
+        <v>138597</v>
+      </c>
+      <c r="E13" s="8">
+        <v>15065</v>
+      </c>
+      <c r="F13" s="7">
+        <v>1565</v>
+      </c>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="8">
+        <v>443</v>
+      </c>
+      <c r="C14" s="8">
+        <v>445</v>
+      </c>
+      <c r="D14" s="8">
+        <v>4331</v>
+      </c>
+      <c r="E14" s="8">
+        <v>15</v>
+      </c>
+      <c r="F14" s="7">
+        <v>780</v>
+      </c>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
completed heuristic_analysis and converted to pdf
</commit_message>
<xml_diff>
--- a/aind_planning_analysis.xlsx
+++ b/aind_planning_analysis.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donay\PycharmProjects\AIND-Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deran/PycharmProjects/AIND-Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="465" windowWidth="29025" windowHeight="20535" tabRatio="841" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="1900" yWindow="480" windowWidth="29020" windowHeight="20540" tabRatio="841" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="stats" sheetId="1" r:id="rId1"/>
@@ -233,8 +233,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -300,7 +300,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -311,6 +311,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -318,22 +320,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="12">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="9"/>
   </cellStyles>
@@ -351,7 +355,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -425,24 +429,24 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>40</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>56</c:v>
+                  <c:v>56.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>180</c:v>
+                  <c:v>180.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.3400000000000001E-2</c:v>
+                  <c:v>0.0234</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B9D5-461C-9974-DF64A83158C8}"/>
             </c:ext>
@@ -502,24 +506,24 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>21</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>84</c:v>
+                  <c:v>84.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.7999999999999997E-3</c:v>
+                  <c:v>0.0098</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-B9D5-461C-9974-DF64A83158C8}"/>
             </c:ext>
@@ -579,24 +583,24 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>55</c:v>
+                  <c:v>55.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>57</c:v>
+                  <c:v>57.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>224</c:v>
+                  <c:v>224.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.39E-2</c:v>
+                  <c:v>0.0339</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-B9D5-461C-9974-DF64A83158C8}"/>
             </c:ext>
@@ -612,11 +616,11 @@
         </c:dLbls>
         <c:gapWidth val="182"/>
         <c:overlap val="100"/>
-        <c:axId val="-2119882656"/>
-        <c:axId val="2126175840"/>
+        <c:axId val="-1410634384"/>
+        <c:axId val="-1410684176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2119882656"/>
+        <c:axId val="-1410634384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -659,7 +663,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126175840"/>
+        <c:crossAx val="-1410684176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -667,7 +671,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2126175840"/>
+        <c:axId val="-1410684176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -718,7 +722,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2119882656"/>
+        <c:crossAx val="-1410634384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -807,7 +811,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -881,24 +885,24 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3343</c:v>
+                  <c:v>3343.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4609</c:v>
+                  <c:v>4609.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30509</c:v>
+                  <c:v>30509.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.772500000000001</c:v>
+                  <c:v>10.7725</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-9973-409E-88AE-DCCCC3D76B10}"/>
             </c:ext>
@@ -958,16 +962,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>624</c:v>
+                  <c:v>624.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>625</c:v>
+                  <c:v>625.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5602</c:v>
+                  <c:v>5602.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>619</c:v>
+                  <c:v>619.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>3.1698</c:v>
@@ -975,7 +979,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-9973-409E-88AE-DCCCC3D76B10}"/>
             </c:ext>
@@ -1035,24 +1039,24 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>4853</c:v>
+                  <c:v>4853.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4855</c:v>
+                  <c:v>4855.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44041</c:v>
+                  <c:v>44041.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.0829000000000004</c:v>
+                  <c:v>8.0829</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-9973-409E-88AE-DCCCC3D76B10}"/>
             </c:ext>
@@ -1068,11 +1072,11 @@
         </c:dLbls>
         <c:gapWidth val="182"/>
         <c:overlap val="100"/>
-        <c:axId val="2127499408"/>
-        <c:axId val="-2115645040"/>
+        <c:axId val="-1410612864"/>
+        <c:axId val="-1410610544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2127499408"/>
+        <c:axId val="-1410612864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1115,7 +1119,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2115645040"/>
+        <c:crossAx val="-1410610544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1123,7 +1127,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2115645040"/>
+        <c:axId val="-1410610544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1174,7 +1178,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127499408"/>
+        <c:crossAx val="-1410612864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1263,7 +1267,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1337,24 +1341,24 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>14663</c:v>
+                  <c:v>14663.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18098</c:v>
+                  <c:v>18098.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>129631</c:v>
+                  <c:v>129631.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>90.786000000000001</c:v>
+                  <c:v>90.786</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-93BE-405D-872F-E470F2B53AB4}"/>
             </c:ext>
@@ -1414,24 +1418,24 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>408</c:v>
+                  <c:v>408.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>409</c:v>
+                  <c:v>409.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3364</c:v>
+                  <c:v>3364.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>392</c:v>
+                  <c:v>392.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3754999999999999</c:v>
+                  <c:v>1.3755</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-93BE-405D-872F-E470F2B53AB4}"/>
             </c:ext>
@@ -1491,24 +1495,24 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>18151</c:v>
+                  <c:v>18151.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18153</c:v>
+                  <c:v>18153.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>159038</c:v>
+                  <c:v>159038.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>33.847200000000001</c:v>
+                  <c:v>33.8472</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-93BE-405D-872F-E470F2B53AB4}"/>
             </c:ext>
@@ -1524,11 +1528,11 @@
         </c:dLbls>
         <c:gapWidth val="182"/>
         <c:overlap val="100"/>
-        <c:axId val="-2121188144"/>
-        <c:axId val="-2121198032"/>
+        <c:axId val="-1410579264"/>
+        <c:axId val="-1410576512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2121188144"/>
+        <c:axId val="-1410579264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1571,7 +1575,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2121198032"/>
+        <c:crossAx val="-1410576512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1579,7 +1583,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2121198032"/>
+        <c:axId val="-1410576512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1630,7 +1634,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2121188144"/>
+        <c:crossAx val="-1410579264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1719,7 +1723,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1793,24 +1797,24 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>41</c:v>
+                  <c:v>41.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43</c:v>
+                  <c:v>43.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>170</c:v>
+                  <c:v>170.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.1499999999999998E-2</c:v>
+                  <c:v>0.0915</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8952-40A1-A24C-CDA39A38DB59}"/>
             </c:ext>
@@ -1870,24 +1874,24 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>48</c:v>
+                  <c:v>48.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.78120000000000001</c:v>
+                  <c:v>0.7812</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8952-40A1-A24C-CDA39A38DB59}"/>
             </c:ext>
@@ -1903,11 +1907,11 @@
         </c:dLbls>
         <c:gapWidth val="182"/>
         <c:overlap val="100"/>
-        <c:axId val="-2116451552"/>
-        <c:axId val="2047309952"/>
+        <c:axId val="-1341743616"/>
+        <c:axId val="-1341741296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2116451552"/>
+        <c:axId val="-1341743616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1950,7 +1954,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2047309952"/>
+        <c:crossAx val="-1341741296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1958,7 +1962,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2047309952"/>
+        <c:axId val="-1341741296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2009,7 +2013,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2116451552"/>
+        <c:crossAx val="-1341743616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2098,7 +2102,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2172,24 +2176,24 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1450</c:v>
+                  <c:v>1450.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1452</c:v>
+                  <c:v>1452.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13303</c:v>
+                  <c:v>13303.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>33.100999999999999</c:v>
+                  <c:v>33.101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-C1A5-4877-8C89-B267C69C1DE1}"/>
             </c:ext>
@@ -2249,24 +2253,24 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>86</c:v>
+                  <c:v>86.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>88</c:v>
+                  <c:v>88.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>841</c:v>
+                  <c:v>841.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>66.970500000000001</c:v>
+                  <c:v>66.9705</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-C1A5-4877-8C89-B267C69C1DE1}"/>
             </c:ext>
@@ -2282,11 +2286,11 @@
         </c:dLbls>
         <c:gapWidth val="182"/>
         <c:overlap val="100"/>
-        <c:axId val="-2115072624"/>
-        <c:axId val="-2115070576"/>
+        <c:axId val="-1410214656"/>
+        <c:axId val="-1410193600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2115072624"/>
+        <c:axId val="-1410214656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2329,7 +2333,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2115070576"/>
+        <c:crossAx val="-1410193600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2337,7 +2341,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2115070576"/>
+        <c:axId val="-1410193600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2388,7 +2392,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2115072624"/>
+        <c:crossAx val="-1410214656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2477,7 +2481,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2551,24 +2555,24 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5038</c:v>
+                  <c:v>5038.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5040</c:v>
+                  <c:v>5040.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44926</c:v>
+                  <c:v>44926.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>181.28120000000001</c:v>
+                  <c:v>181.2812</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-DB31-4DE3-A19B-F557A1F6BAE7}"/>
             </c:ext>
@@ -2628,24 +2632,24 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>293</c:v>
+                  <c:v>293.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>295</c:v>
+                  <c:v>295.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2694</c:v>
+                  <c:v>2694.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>298.95100000000002</c:v>
+                  <c:v>298.951</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-DB31-4DE3-A19B-F557A1F6BAE7}"/>
             </c:ext>
@@ -2661,11 +2665,11 @@
         </c:dLbls>
         <c:gapWidth val="182"/>
         <c:overlap val="100"/>
-        <c:axId val="-2116803936"/>
-        <c:axId val="-2116802160"/>
+        <c:axId val="-1341715056"/>
+        <c:axId val="-1341712304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2116803936"/>
+        <c:axId val="-1341715056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2708,7 +2712,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2116802160"/>
+        <c:crossAx val="-1341712304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2716,7 +2720,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2116802160"/>
+        <c:axId val="-1341712304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2767,7 +2771,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2116803936"/>
+        <c:crossAx val="-1341715056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2856,7 +2860,7 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2925,19 +2929,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-49DC-488B-94DD-C3F7B000309E}"/>
             </c:ext>
@@ -2993,19 +2997,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>8.5377049180327873</c:v>
+                  <c:v>8.537704918032787</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0232168212440711</c:v>
+                  <c:v>2.023216821244071</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6491009547597875</c:v>
+                  <c:v>1.649100954759787</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-49DC-488B-94DD-C3F7B000309E}"/>
             </c:ext>
@@ -3020,11 +3024,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2076116000"/>
-        <c:axId val="-2116075696"/>
+        <c:axId val="-1410121872"/>
+        <c:axId val="-1375296640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2076116000"/>
+        <c:axId val="-1410121872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3067,7 +3071,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2116075696"/>
+        <c:crossAx val="-1375296640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3075,7 +3079,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2116075696"/>
+        <c:axId val="-1375296640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3126,7 +3130,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2076116000"/>
+        <c:crossAx val="-1410121872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3207,7 +3211,7 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3306,19 +3310,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-13BA-4064-8528-AB79025A77D7}"/>
             </c:ext>
@@ -3374,19 +3378,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>33.384615384615387</c:v>
+                  <c:v>33.38461538461539</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.2168020422371777</c:v>
+                  <c:v>6.216802042237177</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.2929196131562137</c:v>
+                  <c:v>3.292919613156214</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-13BA-4064-8528-AB79025A77D7}"/>
             </c:ext>
@@ -3401,11 +3405,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2120690272"/>
-        <c:axId val="-2121760928"/>
+        <c:axId val="-1410557328"/>
+        <c:axId val="-1410555008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2120690272"/>
+        <c:axId val="-1410557328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3448,7 +3452,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2121760928"/>
+        <c:crossAx val="-1410555008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3456,7 +3460,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2121760928"/>
+        <c:axId val="-1410555008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3507,7 +3511,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2120690272"/>
+        <c:crossAx val="-1410557328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3588,7 +3592,7 @@
 </file>
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3612,7 +3616,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>problem3_modified!$A$2</c:f>
+              <c:f>problem3_modified!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3635,7 +3639,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>problem3_modified!$B$1:$E$1</c:f>
+              <c:f>problem3_modified!$H$1:$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -3655,27 +3659,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>problem3_modified!$B$2:$E$2</c:f>
+              <c:f>problem3_modified!$H$2:$K$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.3400000000000001E-2</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.772500000000001</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>90.786000000000001</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3668</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-7B09-4C3D-8F91-FB77DB7C55D4}"/>
             </c:ext>
@@ -3686,7 +3690,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>problem3_modified!$A$3</c:f>
+              <c:f>problem3_modified!$G$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3709,7 +3713,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>problem3_modified!$B$1:$E$1</c:f>
+              <c:f>problem3_modified!$H$1:$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -3729,27 +3733,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>problem3_modified!$B$3:$E$3</c:f>
+              <c:f>problem3_modified!$H$3:$K$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>9.7999999999999997E-3</c:v>
+                  <c:v>0.418803418803419</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.1698</c:v>
+                  <c:v>0.294249245764678</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3754999999999999</c:v>
+                  <c:v>0.0151510144735972</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1565</c:v>
+                  <c:v>0.426663031624864</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-7B09-4C3D-8F91-FB77DB7C55D4}"/>
             </c:ext>
@@ -3760,7 +3764,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>problem3_modified!$A$4</c:f>
+              <c:f>problem3_modified!$G$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3783,7 +3787,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>problem3_modified!$B$1:$E$1</c:f>
+              <c:f>problem3_modified!$H$1:$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -3803,27 +3807,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>problem3_modified!$B$4:$E$4</c:f>
+              <c:f>problem3_modified!$H$4:$K$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.78120000000000001</c:v>
+                  <c:v>33.38461538461539</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>66.970500000000001</c:v>
+                  <c:v>6.216802042237177</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>298.95100000000002</c:v>
+                  <c:v>3.292919613156214</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>780</c:v>
+                  <c:v>0.212649945474373</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-7B09-4C3D-8F91-FB77DB7C55D4}"/>
             </c:ext>
@@ -3838,11 +3842,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="333891992"/>
-        <c:axId val="333898880"/>
+        <c:axId val="-1410541696"/>
+        <c:axId val="-1410539376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="333891992"/>
+        <c:axId val="-1410541696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3885,7 +3889,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="333898880"/>
+        <c:crossAx val="-1410539376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3893,7 +3897,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="333898880"/>
+        <c:axId val="-1410539376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3944,7 +3948,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="333891992"/>
+        <c:crossAx val="-1410541696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3958,6 +3962,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8949,7 +8954,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8985,7 +8990,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9023,7 +9028,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9066,7 +9071,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9104,7 +9109,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9142,7 +9147,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9185,7 +9190,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9226,7 +9231,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9267,7 +9272,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60C8F18B-90CE-49D2-9851-95ADDAA3061E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{60C8F18B-90CE-49D2-9851-95ADDAA3061E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9557,20 +9562,20 @@
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G1" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>16</v>
       </c>
@@ -9596,8 +9601,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B3">
@@ -9625,8 +9630,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="5"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="8"/>
       <c r="B4">
         <v>2</v>
       </c>
@@ -9652,8 +9657,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="5"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="8"/>
       <c r="B5">
         <v>3</v>
       </c>
@@ -9679,8 +9684,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="5"/>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="8"/>
       <c r="B6">
         <v>4</v>
       </c>
@@ -9706,8 +9711,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="5"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="8"/>
       <c r="B7">
         <v>5</v>
       </c>
@@ -9733,8 +9738,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="5"/>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="8"/>
       <c r="B8">
         <v>6</v>
       </c>
@@ -9760,8 +9765,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="5"/>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="8"/>
       <c r="B9">
         <v>7</v>
       </c>
@@ -9787,8 +9792,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="5"/>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="8"/>
       <c r="B10">
         <v>8</v>
       </c>
@@ -9814,8 +9819,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="5"/>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="8"/>
       <c r="B11">
         <v>9</v>
       </c>
@@ -9841,8 +9846,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="5"/>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
       <c r="B12">
         <v>10</v>
       </c>
@@ -9868,7 +9873,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -9876,7 +9881,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>16</v>
       </c>
@@ -9902,8 +9907,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B15">
@@ -9931,8 +9936,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="5"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="8"/>
       <c r="B16">
         <v>2</v>
       </c>
@@ -9947,8 +9952,8 @@
         <v>600</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="5"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="8"/>
       <c r="B17">
         <v>3</v>
       </c>
@@ -9974,8 +9979,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="5"/>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="8"/>
       <c r="B18">
         <v>4</v>
       </c>
@@ -9990,8 +9995,8 @@
         <v>600</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="5"/>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="8"/>
       <c r="B19">
         <v>5</v>
       </c>
@@ -10017,8 +10022,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="5"/>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="8"/>
       <c r="B20">
         <v>6</v>
       </c>
@@ -10033,8 +10038,8 @@
         <v>600</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="5"/>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="8"/>
       <c r="B21">
         <v>7</v>
       </c>
@@ -10060,8 +10065,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="5"/>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="8"/>
       <c r="B22">
         <v>8</v>
       </c>
@@ -10087,8 +10092,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="5"/>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="8"/>
       <c r="B23">
         <v>9</v>
       </c>
@@ -10114,8 +10119,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="5"/>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="8"/>
       <c r="B24">
         <v>10</v>
       </c>
@@ -10141,7 +10146,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -10149,7 +10154,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>16</v>
       </c>
@@ -10175,8 +10180,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="5" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
         <v>28</v>
       </c>
       <c r="B27">
@@ -10204,8 +10209,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="5"/>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="8"/>
       <c r="B28">
         <v>2</v>
       </c>
@@ -10220,8 +10225,8 @@
         <v>600</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="5"/>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="8"/>
       <c r="B29">
         <v>3</v>
       </c>
@@ -10247,8 +10252,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="5"/>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="8"/>
       <c r="B30">
         <v>4</v>
       </c>
@@ -10263,8 +10268,8 @@
         <v>600</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="5"/>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="8"/>
       <c r="B31">
         <v>5</v>
       </c>
@@ -10290,8 +10295,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="5"/>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="8"/>
       <c r="B32">
         <v>6</v>
       </c>
@@ -10306,8 +10311,8 @@
         <v>600</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="5"/>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="8"/>
       <c r="B33">
         <v>7</v>
       </c>
@@ -10333,8 +10338,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="5"/>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="8"/>
       <c r="B34">
         <v>8</v>
       </c>
@@ -10360,8 +10365,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="5"/>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="8"/>
       <c r="B35">
         <v>9</v>
       </c>
@@ -10387,8 +10392,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="5"/>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="8"/>
       <c r="B36">
         <v>10</v>
       </c>
@@ -10433,14 +10438,14 @@
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -10466,7 +10471,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -10492,7 +10497,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -10518,7 +10523,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -10544,7 +10549,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -10552,7 +10557,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -10560,7 +10565,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -10568,7 +10573,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -10589,17 +10594,17 @@
       <selection activeCell="F1" sqref="A1:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
@@ -10619,7 +10624,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -10639,7 +10644,7 @@
         <v>2.3400000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -10659,7 +10664,7 @@
         <v>9.7999999999999997E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -10679,7 +10684,7 @@
         <v>3.39E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -10687,7 +10692,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -10695,7 +10700,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -10703,7 +10708,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -10723,7 +10728,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
@@ -10743,7 +10748,7 @@
         <v>10.772500000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
@@ -10763,7 +10768,7 @@
         <v>3.1698</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
@@ -10783,7 +10788,7 @@
         <v>8.0829000000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -10791,7 +10796,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -10799,7 +10804,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -10807,7 +10812,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
@@ -10827,7 +10832,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>0</v>
       </c>
@@ -10847,7 +10852,7 @@
         <v>90.786000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
@@ -10867,7 +10872,7 @@
         <v>1.3754999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>4</v>
       </c>
@@ -10901,17 +10906,17 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
@@ -10931,7 +10936,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>59</v>
       </c>
@@ -10951,7 +10956,7 @@
         <v>9.1499999999999998E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>60</v>
       </c>
@@ -10971,7 +10976,7 @@
         <v>0.78120000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -10979,7 +10984,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -10987,7 +10992,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -10995,7 +11000,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -11003,7 +11008,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -11011,7 +11016,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
@@ -11031,7 +11036,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>59</v>
       </c>
@@ -11051,7 +11056,7 @@
         <v>33.100999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>60</v>
       </c>
@@ -11071,7 +11076,7 @@
         <v>66.970500000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -11079,7 +11084,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -11087,7 +11092,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -11095,7 +11100,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -11103,7 +11108,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -11123,7 +11128,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>59</v>
       </c>
@@ -11143,7 +11148,7 @@
         <v>181.28120000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>60</v>
       </c>
@@ -11177,13 +11182,13 @@
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>61</v>
       </c>
@@ -11203,7 +11208,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>59</v>
       </c>
@@ -11233,7 +11238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>60</v>
       </c>
@@ -11277,13 +11282,13 @@
       <selection activeCell="D2" sqref="B2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>61</v>
       </c>
@@ -11303,7 +11308,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -11329,7 +11334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>60</v>
       </c>
@@ -11369,386 +11374,386 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="E4" sqref="A2:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="19.25" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9" style="6"/>
+    <col min="1" max="1" width="19.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7" t="s">
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
     </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="7">
         <v>2.3400000000000001E-2</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>10.772500000000001</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="7">
         <v>90.786000000000001</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <v>3668</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="6"/>
+      <c r="G2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="7">
         <v>1</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="7">
         <v>1</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2" s="7">
         <v>1</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="6">
         <v>1</v>
       </c>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>9.7999999999999997E-3</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>3.1698</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <v>1.3754999999999999</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>1565</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7" t="s">
+      <c r="F3" s="6"/>
+      <c r="G3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="7">
         <f>B3/B2</f>
         <v>0.41880341880341876</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="7">
         <f t="shared" ref="I3:K3" si="0">C3/C2</f>
         <v>0.29424924576467854</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="7">
         <f t="shared" si="0"/>
         <v>1.5151014473597249E-2</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="7">
         <f t="shared" si="0"/>
         <v>0.42666303162486369</v>
       </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
     </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>0.78120000000000001</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>66.970500000000001</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>298.95100000000002</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <v>780</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7" t="s">
+      <c r="F4" s="6"/>
+      <c r="G4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="7">
         <f>B4/B2</f>
         <v>33.384615384615387</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="7">
         <f t="shared" ref="I4:K4" si="1">C4/C2</f>
         <v>6.2168020422371777</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="7">
         <f t="shared" si="1"/>
         <v>3.2929196131562137</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K4" s="7">
         <f t="shared" si="1"/>
         <v>0.21264994547437296</v>
       </c>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
     </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
     </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
     </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
     </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
     </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
     </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A12" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="7">
         <v>112090</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>121416</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="7">
         <v>1055564</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="7">
         <v>15</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <v>3668</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A13" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="7">
         <v>15450</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="7">
         <v>15451</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="7">
         <v>138597</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="7">
         <v>15065</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="6">
         <v>1565</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
     </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="7" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A14" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="7">
         <v>443</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="7">
         <v>445</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="7">
         <v>4331</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="7">
         <v>15</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="6">
         <v>780</v>
       </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
     </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
     </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>